<commit_message>
Verify Page Title added for Smoke Suite
</commit_message>
<xml_diff>
--- a/Test-Data/EMICalculatorTestData.xlsx
+++ b/Test-Data/EMICalculatorTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse Oxygen\EMICalculator\Test-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279AEA3D-749E-4BD7-B32A-DFD2BE8D3312}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E64DB0C-98DF-4FC3-BAA4-9347C997E127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{92E2F852-BD6B-41ED-A4B5-D8E9A05A7144}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>emiCalculator</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>LoanTenure</t>
+  </si>
+  <si>
+    <t>driverTitleTestData</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>EMI Calculator for Home Loan, Car Loan &amp; Personal Loan in India</t>
   </si>
 </sst>
 </file>
@@ -421,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECAF94B-428D-49D9-9472-74E7329DAEEE}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,12 +477,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A3" xr:uid="{2CFA6190-8856-47DD-9E1E-4DC28784C65E}"/>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{00102529-4383-405C-991C-39FA5A1433F1}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{B4977808-D761-4BB8-95BD-5C190B91FAA0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
isElementPresent() and verifyTotalPaymentAmount() tests added under smoke suite
</commit_message>
<xml_diff>
--- a/Test-Data/EMICalculatorTestData.xlsx
+++ b/Test-Data/EMICalculatorTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse Oxygen\EMICalculator\Test-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E64DB0C-98DF-4FC3-BAA4-9347C997E127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA96FE78-51A2-4D07-AB5C-A7F2FA0D50DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{92E2F852-BD6B-41ED-A4B5-D8E9A05A7144}"/>
+    <workbookView xWindow="5760" yWindow="3432" windowWidth="17280" windowHeight="9072" xr2:uid="{92E2F852-BD6B-41ED-A4B5-D8E9A05A7144}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanDetails" sheetId="1" r:id="rId1"/>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>emiCalculator</t>
   </si>
   <si>
-    <t>WebPageURL</t>
-  </si>
-  <si>
-    <t>https://www.emicalculator.net</t>
-  </si>
-  <si>
     <t>CarLoanAmount</t>
   </si>
   <si>
@@ -61,24 +55,22 @@
   </si>
   <si>
     <t>EMI Calculator for Home Loan, Car Loan &amp; Personal Loan in India</t>
+  </si>
+  <si>
+    <t>totalPaymentAmountVerify</t>
+  </si>
+  <si>
+    <t>expectedTotalAmount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,17 +99,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECAF94B-428D-49D9-9472-74E7329DAEEE}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,7 +431,7 @@
     <col min="1" max="1" width="39.44140625" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -450,61 +440,78 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+      <c r="A3">
+        <v>1500000</v>
       </c>
       <c r="B3">
-        <v>1500000</v>
+        <v>9.5</v>
       </c>
       <c r="C3">
-        <v>9.5</v>
-      </c>
-      <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1000000</v>
+      </c>
+      <c r="B11">
+        <v>12.5</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1349876</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:A3" xr:uid="{2CFA6190-8856-47DD-9E1E-4DC28784C65E}"/>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{00102529-4383-405C-991C-39FA5A1433F1}"/>
-    <hyperlink ref="A7" r:id="rId2" xr:uid="{B4977808-D761-4BB8-95BD-5C190B91FAA0}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Valid Input Test added. reports directory updated
</commit_message>
<xml_diff>
--- a/Test-Data/EMICalculatorTestData.xlsx
+++ b/Test-Data/EMICalculatorTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse Oxygen\EMICalculator\Test-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA96FE78-51A2-4D07-AB5C-A7F2FA0D50DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B83D1A-76F5-4071-A1EF-324F1032AE5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3432" windowWidth="17280" windowHeight="9072" xr2:uid="{92E2F852-BD6B-41ED-A4B5-D8E9A05A7144}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{92E2F852-BD6B-41ED-A4B5-D8E9A05A7144}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanDetails" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>emiCalculator</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>expectedTotalAmount</t>
+  </si>
+  <si>
+    <t>verifyDataValues</t>
+  </si>
+  <si>
+    <t>qwerty</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECAF94B-428D-49D9-9472-74E7329DAEEE}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,6 +515,33 @@
         <v>1349876</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A3" xr:uid="{2CFA6190-8856-47DD-9E1E-4DC28784C65E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>